<commit_message>
bổ sung chú thích
</commit_message>
<xml_diff>
--- a/lophoc.xlsx
+++ b/lophoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\OneDrive - Industrial University of HoChiMinh City\TEACHING\IUH\IUH.PTDL\LT\LT-PTDL-new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Subject\Year 3\Phân tích dữ liệu\DataOfDuc\nmptdlai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E680739-8B6C-4A05-921C-AE2C8798FE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F80126A-F0D3-4CD1-9E44-2C564B85582A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -45,16 +45,16 @@
     <t>nắng</t>
   </si>
   <si>
-    <t>có</t>
-  </si>
-  <si>
-    <t>không</t>
-  </si>
-  <si>
     <t>Sức khỏe</t>
   </si>
   <si>
     <t>tốt</t>
+  </si>
+  <si>
+    <t>nghỉ</t>
+  </si>
+  <si>
+    <t>học</t>
   </si>
 </sst>
 </file>
@@ -375,19 +375,19 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -396,7 +396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -404,10 +404,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -415,10 +415,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -426,10 +426,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -437,40 +437,40 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>